<commit_message>
Add stage-1 tasks: A1 - A6
</commit_message>
<xml_diff>
--- a/pinosu/evidence.xlsx
+++ b/pinosu/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinos\dev\gon-evidence\pinosu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinos\OneDrive\Desktop\gon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BF322E-E967-477E-9206-24F15FDF1A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F149DABA-E3A8-4C55-AAD1-74A7D360800D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="3390" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="3315" windowWidth="21600" windowHeight="11295" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t>TeamName</t>
   </si>
@@ -76,33 +76,15 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
     <t>nft id</t>
   </si>
   <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
     <t>ibc class on chain</t>
   </si>
   <si>
@@ -143,13 +125,55 @@
   </si>
   <si>
     <t>Pino' | Confio#6925</t>
+  </si>
+  <si>
+    <t>864BF840BB4B27F07708E80565052FA675E05CAACAA0E9A66DEA4B5CD5C4EB09</t>
+  </si>
+  <si>
+    <t>pizza2023</t>
+  </si>
+  <si>
+    <t>24778DF14F3C0CEE12898C1A2E36A0CA1DD030BC3F22AAC42A5F896BD2AA827B</t>
+  </si>
+  <si>
+    <t>margherita</t>
+  </si>
+  <si>
+    <t>045C3628385C34759DEBDEA111FD6F647CC951E2CADAEDB77077512D9DC98CA9</t>
+  </si>
+  <si>
+    <t>marinara</t>
+  </si>
+  <si>
+    <t>B0B21A63C473404EA933EEEF8FC1C4A09EA6D633BD903F344CA0963E0296801C</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>821B1A882B4CDFE5C71D1207C1FB9A6FAF3C0AD468116FCA624134132DFE8381</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>juno1peuf6njez4e0mnq2ucshvq5u3n7p4llg05sww8cmzlpreawdpujs2pe3k6</t>
+  </si>
+  <si>
+    <t>ibc/43A4BD364067EB619788A846CF464821CDA7F24C1D242F7DC322A930B1455EC9</t>
+  </si>
+  <si>
+    <t>CB3CA4693E67861D95F7B67BEFA51071BFE3C966E218205FD17F0B159A555D21</t>
+  </si>
+  <si>
+    <t>8D1524266C33950850116EF8BDD573CA1B4B59BC73E534B844BEB5BEAEBA058E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -167,6 +191,17 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -201,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -210,6 +245,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -598,28 +634,28 @@
     </row>
     <row r="2" spans="1:8" ht="14.25">
       <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="F2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -644,15 +680,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -677,15 +713,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -710,15 +746,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -743,15 +779,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -776,25 +812,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -819,25 +855,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -862,25 +898,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -905,25 +941,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -948,25 +984,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -991,25 +1027,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1022,7 +1058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1039,10 +1077,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1067,25 +1105,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1110,25 +1148,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1152,12 +1190,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1187,12 +1225,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1222,12 +1260,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1257,12 +1295,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1277,9 +1315,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1295,23 +1335,35 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.25">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1319,7 +1371,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1335,24 +1389,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1365,7 +1419,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1381,24 +1437,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1411,7 +1467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1427,24 +1485,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
+      <c r="A2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1457,7 +1515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1475,24 +1535,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1517,15 +1577,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1550,17 +1610,17 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>